<commit_message>
ch 1, 2 and debug appendix
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44893</v>
+        <v>44914</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44892</v>
+        <v>44913</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44891</v>
+        <v>44912</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44890</v>
+        <v>44911</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44889</v>
+        <v>44910</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44888</v>
+        <v>44909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ch 1 and 2 final Lisa edits
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44914</v>
+        <v>44916</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44913</v>
+        <v>44915</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44912</v>
+        <v>44914</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44911</v>
+        <v>44913</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44910</v>
+        <v>44912</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44909</v>
+        <v>44911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ch 4 exercise plot typo
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44959</v>
+        <v>44974</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44958</v>
+        <v>44973</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44957</v>
+        <v>44972</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44956</v>
+        <v>44971</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44955</v>
+        <v>44970</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44954</v>
+        <v>44969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CH 4 and glossary stuff
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>45337</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>45336</v>
+        <v>45370</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>45335</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>45334</v>
+        <v>45368</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>45333</v>
+        <v>45367</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>45332</v>
+        <v>45366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>